<commit_message>
PQ 106 has been added(Lambda Solution).
</commit_message>
<xml_diff>
--- a/Excel Files/PQ Challenges/PQ Challenge 105 Problem.xlsx
+++ b/Excel Files/PQ Challenges/PQ Challenge 105 Problem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\Excel-BI-Python\Excel Files\PQ Challenges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942C43AB-83D9-4D1F-98FE-E6CD78068963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CC78E5-A6A2-4BAC-B11F-9C8D2DDB50EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="34580" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,7 +108,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\.hh:mm:ss"/>
-    <numFmt numFmtId="169" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -314,7 +314,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -937,7 +937,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="1656" row="12">
+  <wetp:taskpane dockstate="right" visibility="0" width="1615" row="12">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -955,6 +955,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -967,10 +970,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1161,6 +1164,34 @@
       </c>
       <c r="J7" t="str">
         <v>3.03:23:00</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H13" t="str" cm="1">
+        <f t="array" ref="H13">_xlfn.LAMBDA(_xlpm.Text,_xlpm.AddPart,
+        _xlfn.LET(
+            _xlpm.Text2, A5,
+            _xlpm.AddPart2, B5,
+            _xlpm.Splitted, _xlfn.WRAPROWS(_xlfn.TEXTSPLIT(_xlpm.Text, " "), 2),
+            _xlpm.MappedData, _xlfn.MAP(
+                {"Day","Hour","Minute","Second"},
+                _xlfn.LAMBDA(_xlpm.a,
+                    _xlfn.LET(
+                        _xlpm.Length, LEN(_xlpm.a),
+                        _xlpm.InTextTime, IFERROR(
+                            INDEX(_xlfn._xlws.FILTER(_xlfn.CHOOSECOLS(_xlpm.Splitted, 1), PROPER(LEFT(_xlfn.CHOOSECOLS(_xlpm.Splitted, 2), _xlpm.Length)) = _xlpm.a), 1, 1) *
+                                1,
+                            0
+                        ),
+                        _xlpm.InAddPart, IF(PROPER(LEFT(_xlfn.TEXTAFTER(_xlpm.AddPart, " "), _xlpm.Length)) = _xlpm.a, _xlfn.TEXTBEFORE(_xlpm.AddPart, " ") * 1, 0),
+                        _xlpm.InTextTime + _xlpm.InAddPart
+                    )
+                )
+            ),
+            TEXT(SUM(_xlpm.MappedData / {1,24,1440,86400}), "d.hh:mm:ss")
+        )
+    )(A5,B5)</f>
+        <v>0.04:15:22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>